<commit_message>
Included Test Data Report
</commit_message>
<xml_diff>
--- a/AdactinTestData.xlsx
+++ b/AdactinTestData.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karthik\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karthik\Desktop\Eclipse Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="AdultsperRoom">Sheet2!$E$2:$E$5</definedName>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
   <si>
     <t>Browser</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>Super Deluxe</t>
+  </si>
+  <si>
+    <t>999</t>
   </si>
 </sst>
 </file>
@@ -250,7 +253,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -286,39 +289,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -332,6 +310,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -647,231 +629,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="6"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="C8" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C9" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C10" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2">
+      <c r="C11" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="2">
+      <c r="C12" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="6" t="str">
-        <f>UPPER(A15)</f>
-        <v>BOOK A HOTEL</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C13" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="4">
+      <c r="C16" s="8">
         <v>1234132412341320</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="2">
+      <c r="C18" s="8">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="2">
+      <c r="C19" s="8">
         <v>2022</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="2">
-        <v>777</v>
+      <c r="C20" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A15:B15"/>
-  </mergeCells>
   <dataValidations count="9">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
       <formula1>Location</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6">
       <formula1>Hotels</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
       <formula1>RoomType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
       <formula1>NumberofRooms</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
       <formula1>AdultsperRoom</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
       <formula1>ChildrenperRoom</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17">
       <formula1>CreditCardType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18">
       <formula1>ExpiryMonth</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19">
       <formula1>ExpiryYear</formula1>
     </dataValidation>
   </dataValidations>
@@ -884,299 +850,299 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11" style="9"/>
+    <col min="1" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="6">
         <v>1</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="6">
         <v>1</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="6">
         <v>0</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="6">
         <v>1</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="6">
         <v>2011</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="6">
         <v>2</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="6">
         <v>2</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="6">
         <v>1</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="6">
         <v>2</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="6">
         <v>2012</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="6">
         <v>3</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="6">
         <v>3</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="6">
         <v>2</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="6">
         <v>3</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="6">
         <v>2013</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="6">
         <v>4</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="6">
         <v>4</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="6">
         <v>3</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="6">
         <v>4</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="6">
         <v>2014</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6">
         <v>5</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6">
         <v>4</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10">
+      <c r="G6" s="6"/>
+      <c r="H6" s="6">
         <v>5</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="6">
         <v>2015</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6">
         <v>6</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6">
         <v>6</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="6">
         <v>2016</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6">
         <v>7</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6">
         <v>7</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="6">
         <v>2017</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6">
         <v>8</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10">
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6">
         <v>8</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="6">
         <v>2018</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6">
         <v>9</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10">
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6">
         <v>9</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="6">
         <v>2019</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6">
         <v>10</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10">
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6">
         <v>10</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="6">
         <v>2020</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6">
         <v>11</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="6">
         <v>2021</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6">
         <v>12</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="6">
         <v>2022</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Boni updated in baseclass
</commit_message>
<xml_diff>
--- a/AdactinTestData.xlsx
+++ b/AdactinTestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karthik\Desktop\Eclipse Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karthik\git\Adactin\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97E197C-950E-4EBA-ABBA-64C333E89F73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
+    <workbookView xWindow="5115" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,15 +54,9 @@
     <t>User Name</t>
   </si>
   <si>
-    <t>PavithraN</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
-    <t>Pavi@2426</t>
-  </si>
-  <si>
     <t>TEST DATA</t>
   </si>
   <si>
@@ -195,12 +190,18 @@
   </si>
   <si>
     <t>999</t>
+  </si>
+  <si>
+    <t>karthik18</t>
+  </si>
+  <si>
+    <t>LXCW11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -628,11 +629,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +645,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -666,47 +667,47 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="8">
         <v>2</v>
@@ -714,23 +715,23 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="8">
         <v>2</v>
@@ -738,7 +739,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" s="8">
         <v>0</v>
@@ -746,34 +747,34 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16" s="8">
         <v>1234132412341320</v>
@@ -781,15 +782,15 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" s="8">
         <v>6</v>
@@ -797,7 +798,7 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C19" s="8">
         <v>2022</v>
@@ -805,39 +806,39 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="9">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Location</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>Hotels</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>RoomType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>NumberofRooms</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>AdultsperRoom</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>ChildrenperRoom</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>CreditCardType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>ExpiryMonth</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>ExpiryYear</formula1>
     </dataValidation>
   </dataValidations>
@@ -847,7 +848,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -861,42 +862,42 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="I1" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="D2" s="6">
         <v>1</v>
@@ -908,7 +909,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H2" s="6">
         <v>1</v>
@@ -919,13 +920,13 @@
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" s="6">
         <v>2</v>
@@ -937,7 +938,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H3" s="6">
         <v>2</v>
@@ -948,13 +949,13 @@
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D4" s="6">
         <v>3</v>
@@ -966,7 +967,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H4" s="6">
         <v>3</v>
@@ -977,13 +978,13 @@
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" s="6">
         <v>4</v>
@@ -995,7 +996,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H5" s="6">
         <v>4</v>
@@ -1006,7 +1007,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1027,7 +1028,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1046,7 +1047,7 @@
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1065,7 +1066,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>

</xml_diff>